<commit_message>
Ajouts images déprt CLMI Cité de l'Or
</commit_message>
<xml_diff>
--- a/excel/ardoise_info_neutre.xlsx
+++ b/excel/ardoise_info_neutre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinebeausoleil/Documents/TourAbitibi/Guide/guide2024/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358E30E3-C84E-1E48-B8A5-38EC57CE7491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC0E30F-7667-E54D-8AEB-101E02B4CCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="9700" windowWidth="26360" windowHeight="8300" activeTab="3" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="25620" yWindow="560" windowWidth="51140" windowHeight="28180" activeTab="2" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="COORD" sheetId="1" r:id="rId1"/>
@@ -122,9 +122,6 @@
     <t>Pier.luc.pol@gmail.com</t>
   </si>
   <si>
-    <t>(819) 442-1522</t>
-  </si>
-  <si>
     <t>Esteban Guevin</t>
   </si>
   <si>
@@ -134,24 +131,12 @@
     <t>estebanguevin@gmail.com</t>
   </si>
   <si>
-    <t>Mécano 1 + gestion du projet sur place</t>
-  </si>
-  <si>
     <t>Conducteur</t>
   </si>
   <si>
     <t>Mécano 2</t>
   </si>
   <si>
-    <t>Mathieu St-Laurent</t>
-  </si>
-  <si>
-    <t>450-522-7775</t>
-  </si>
-  <si>
-    <t>mathieustlaurent@icloud.com</t>
-  </si>
-  <si>
     <t>Issac Bonequi</t>
   </si>
   <si>
@@ -162,6 +147,21 @@
   </si>
   <si>
     <t>Mecano</t>
+  </si>
+  <si>
+    <t>Stephan Couture</t>
+  </si>
+  <si>
+    <t>Stefquattro@yahoo.ca</t>
+  </si>
+  <si>
+    <t>514-518-7507</t>
+  </si>
+  <si>
+    <t>Mécano 1 + gestion équipe dépannage neutre</t>
+  </si>
+  <si>
+    <t>819-442-1522</t>
   </si>
 </sst>
 </file>
@@ -240,7 +240,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -249,49 +249,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -364,34 +324,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -405,12 +341,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -418,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -444,29 +378,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -474,6 +401,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -490,10 +423,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -991,10 +920,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EDA790-0658-EF4E-9D2F-BE0EFC66A120}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1002,7 +931,7 @@
     <col min="1" max="1" width="23.5" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="4" width="37.83203125" customWidth="1"/>
+    <col min="4" max="4" width="43.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1026,76 +955,76 @@
       <c r="B2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="20" t="s">
         <v>40</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="D3" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="10"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D12" s="26"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="19"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{8FBE4E08-0305-AA42-8561-C40A1424DEA8}"/>
-    <hyperlink ref="B4" r:id="rId2" display="mailto:mathieustlaurent@icloud.com" xr:uid="{D7BA11A6-E9BC-D34B-A25A-0159996846A0}"/>
-    <hyperlink ref="B5" r:id="rId3" display="mailto:isaacbonequi@atelierolympia.com" xr:uid="{6675C248-0D43-7F44-BD56-7B1B2B558FC0}"/>
+    <hyperlink ref="B4" r:id="rId2" display="mailto:isaacbonequi@atelierolympia.com" xr:uid="{6675C248-0D43-7F44-BD56-7B1B2B558FC0}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{B7A5C3F4-F0D2-E747-B722-C58D0D1A3E80}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1106,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A4AC57-2E28-5943-8E7B-8ACE99136666}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1121,206 +1050,206 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="25"/>
+      <c r="B2" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="11" t="str">
+      <c r="B3" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="12" t="str">
         <f>C2</f>
-        <v>Mathieu St-Laurent</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="13"/>
+        <v>Stephan Couture</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
-        <v>3</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="11" t="str">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="12" t="str">
         <f t="shared" ref="C4:C8" si="0">C3</f>
-        <v>Mathieu St-Laurent</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="23" t="s">
+        <v>Stephan Couture</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="11" t="str">
+      <c r="B5" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>Mathieu St-Laurent</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="13"/>
+        <v>Stephan Couture</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="11" t="str">
+      <c r="B6" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>Mathieu St-Laurent</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="13"/>
+        <v>Stephan Couture</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="11" t="str">
+      <c r="B7" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>Mathieu St-Laurent</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="24" t="s">
+        <v>Stephan Couture</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="13"/>
+      <c r="G7" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="11" t="str">
+      <c r="B8" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>Mathieu St-Laurent</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="24" t="s">
+        <v>Stephan Couture</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="15"/>
+      <c r="G8" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1330,13 +1259,13 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2FF631A4-0570-384A-95CA-9C4F7FFE55C4}">
           <x14:formula1>
-            <xm:f>COORD_DEP!$A$2:$A$18</xm:f>
+            <xm:f>COORD_DEP!$A$2:$A$17</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G8 B2:E8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{58D354B3-A020-544F-A500-46EE14A63744}">
           <x14:formula1>
-            <xm:f>COORD_DEP!$A$2:$A$15</xm:f>
+            <xm:f>COORD_DEP!$A$2:$A$14</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F8</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
MAJ staff et signalisation
</commit_message>
<xml_diff>
--- a/excel/ardoise_info_neutre.xlsx
+++ b/excel/ardoise_info_neutre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC0E30F-7667-E54D-8AEB-101E02B4CCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DDDDEF-73A1-5548-AF73-443FBE9FB621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25620" yWindow="560" windowWidth="51140" windowHeight="28180" activeTab="2" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="25620" yWindow="560" windowWidth="51140" windowHeight="28180" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="COORD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="44">
   <si>
     <t>Bruno Gauthier</t>
   </si>
@@ -162,13 +162,22 @@
   </si>
   <si>
     <t>819-442-1522</t>
+  </si>
+  <si>
+    <t>William Baril</t>
+  </si>
+  <si>
+    <t>\(819) 290-0096</t>
+  </si>
+  <si>
+    <t>william.baril@assnat.qc.ca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +240,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF050505"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -352,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -407,6 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -722,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72262817-9D66-6D48-97C4-5126E8F8BB18}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -779,11 +795,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="cloeparadis@gmail.com" xr:uid="{8E818DE4-AC70-4447-901D-595586C5B976}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{F460A2CC-A819-E144-832F-1FA2B437848F}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{F1C9372A-B77E-4D44-A286-658ED7B416FB}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{41A37541-D021-B845-9DF3-E6222462AF05}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -795,7 +823,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -922,7 +950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EDA790-0658-EF4E-9D2F-BE0EFC66A120}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Compil - modif staff
</commit_message>
<xml_diff>
--- a/excel/ardoise_info_neutre.xlsx
+++ b/excel/ardoise_info_neutre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DDDDEF-73A1-5548-AF73-443FBE9FB621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C2037A-9DF8-B14C-A52F-472478EA135C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25620" yWindow="560" windowWidth="51140" windowHeight="28180" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="45">
   <si>
     <t>Bruno Gauthier</t>
   </si>
@@ -146,9 +146,6 @@
     <t>isaacbonequi@atelierolympia.com</t>
   </si>
   <si>
-    <t>Mecano</t>
-  </si>
-  <si>
     <t>Stephan Couture</t>
   </si>
   <si>
@@ -164,13 +161,19 @@
     <t>819-442-1522</t>
   </si>
   <si>
-    <t>William Baril</t>
-  </si>
-  <si>
-    <t>\(819) 290-0096</t>
-  </si>
-  <si>
-    <t>william.baril@assnat.qc.ca</t>
+    <t>Guillaume Julien</t>
+  </si>
+  <si>
+    <t>Mécano 3</t>
+  </si>
+  <si>
+    <t>Mecano 3</t>
+  </si>
+  <si>
+    <t>gjulien18@hotmail.com</t>
+  </si>
+  <si>
+    <t>819-860-4596</t>
   </si>
 </sst>
 </file>
@@ -741,7 +744,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,22 +799,14 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>42</v>
-      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="cloeparadis@gmail.com" xr:uid="{8E818DE4-AC70-4447-901D-595586C5B976}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{F460A2CC-A819-E144-832F-1FA2B437848F}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{F1C9372A-B77E-4D44-A286-658ED7B416FB}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{41A37541-D021-B845-9DF3-E6222462AF05}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -951,7 +946,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -984,10 +979,10 @@
         <v>26</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1001,7 +996,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1020,20 +1015,31 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="23" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>38</v>
       </c>
       <c r="D5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="10"/>
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D11" s="19"/>
@@ -1053,6 +1059,7 @@
     <hyperlink ref="B3" r:id="rId1" xr:uid="{8FBE4E08-0305-AA42-8561-C40A1424DEA8}"/>
     <hyperlink ref="B4" r:id="rId2" display="mailto:isaacbonequi@atelierolympia.com" xr:uid="{6675C248-0D43-7F44-BD56-7B1B2B558FC0}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{B7A5C3F4-F0D2-E747-B722-C58D0D1A3E80}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{2A67B08B-D29D-E243-91F2-028779F3CB0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1064,7 +1071,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1118,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>32</v>
@@ -1120,7 +1127,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>3</v>
@@ -1197,7 +1204,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>3</v>
@@ -1222,7 +1229,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Compil - modif staff et nb équipes sprint
</commit_message>
<xml_diff>
--- a/excel/ardoise_info_neutre.xlsx
+++ b/excel/ardoise_info_neutre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C2037A-9DF8-B14C-A52F-472478EA135C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EE0370-6363-C848-8150-754411E16381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25620" yWindow="560" windowWidth="51140" windowHeight="28180" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="25620" yWindow="560" windowWidth="51140" windowHeight="28180" activeTab="2" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="COORD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
   <si>
     <t>Bruno Gauthier</t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>819-860-4596</t>
+  </si>
+  <si>
+    <t>Patrick Trépannier</t>
+  </si>
+  <si>
+    <t>patrickt1@hotmail.com</t>
+  </si>
+  <si>
+    <t>819-649-1250</t>
   </si>
 </sst>
 </file>
@@ -743,7 +752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72262817-9D66-6D48-97C4-5126E8F8BB18}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -945,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EDA790-0658-EF4E-9D2F-BE0EFC66A120}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1038,6 +1047,20 @@
         <v>44</v>
       </c>
       <c r="D6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1071,7 +1094,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1152,7 +1175,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Correction staff et locaux
</commit_message>
<xml_diff>
--- a/excel/ardoise_info_neutre.xlsx
+++ b/excel/ardoise_info_neutre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EE0370-6363-C848-8150-754411E16381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C7432B-3E4C-8945-96CE-408C608D6C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25620" yWindow="560" windowWidth="51140" windowHeight="28180" activeTab="2" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="25620" yWindow="560" windowWidth="51140" windowHeight="28180" activeTab="1" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="COORD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="53">
   <si>
     <t>Bruno Gauthier</t>
   </si>
@@ -179,10 +179,25 @@
     <t>Patrick Trépannier</t>
   </si>
   <si>
-    <t>patrickt1@hotmail.com</t>
-  </si>
-  <si>
     <t>819-649-1250</t>
+  </si>
+  <si>
+    <t>Antoine St-Jean</t>
+  </si>
+  <si>
+    <t>Stéphan Larose</t>
+  </si>
+  <si>
+    <t>stephan.larose@ville.valdor.qc.ca</t>
+  </si>
+  <si>
+    <t>\(819) 856-1565</t>
+  </si>
+  <si>
+    <t>releve@tourabitibi.qc.ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patrickt1@hotmail.com </t>
   </si>
 </sst>
 </file>
@@ -750,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72262817-9D66-6D48-97C4-5126E8F8BB18}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -808,14 +823,32 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="B5" s="5"/>
+      <c r="A5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C5" s="30"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="cloeparadis@gmail.com" xr:uid="{8E818DE4-AC70-4447-901D-595586C5B976}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{F460A2CC-A819-E144-832F-1FA2B437848F}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{F1C9372A-B77E-4D44-A286-658ED7B416FB}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{BD6180F8-7D3F-224E-AD03-CC55A4456DE0}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{D7A2B01D-7E39-A149-9EE4-136CBCD13BFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -826,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C2AAB0-2148-A34F-B523-8D7C783C697A}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -860,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -871,7 +904,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -907,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -918,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -929,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -954,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EDA790-0658-EF4E-9D2F-BE0EFC66A120}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1054,11 +1087,11 @@
       <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>46</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>47</v>
       </c>
       <c r="D7" t="s">
         <v>41</v>
@@ -1083,6 +1116,7 @@
     <hyperlink ref="B4" r:id="rId2" display="mailto:isaacbonequi@atelierolympia.com" xr:uid="{6675C248-0D43-7F44-BD56-7B1B2B558FC0}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{B7A5C3F4-F0D2-E747-B722-C58D0D1A3E80}"/>
     <hyperlink ref="B6" r:id="rId4" xr:uid="{2A67B08B-D29D-E243-91F2-028779F3CB0B}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{C0513BE5-67C0-B546-BA21-D1F1FAFBBD5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>